<commit_message>
Add mini hooks to BOM
</commit_message>
<xml_diff>
--- a/hardware/probes/BOM.xlsx
+++ b/hardware/probes/BOM.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>Part</t>
   </si>
@@ -70,6 +70,27 @@
   </si>
   <si>
     <t>DigiKey: http://www.digikey.com/product-search/en?keywords=086sc-2401</t>
+  </si>
+  <si>
+    <t>Mini Hook Black</t>
+  </si>
+  <si>
+    <t>Mini Hook Red</t>
+  </si>
+  <si>
+    <t>E-Z-Hook</t>
+  </si>
+  <si>
+    <t>XR25RED</t>
+  </si>
+  <si>
+    <t>XR25BLK</t>
+  </si>
+  <si>
+    <t>https://octopart.com/xr25blk-e-z-hook-19790456</t>
+  </si>
+  <si>
+    <t>https://octopart.com/xr25red-e-z-hook-19790462</t>
   </si>
 </sst>
 </file>
@@ -410,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -486,13 +507,43 @@
         <v>16</v>
       </c>
     </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D4" r:id="rId1"/>
     <hyperlink ref="D3" r:id="rId2"/>
     <hyperlink ref="D2" r:id="rId3"/>
+    <hyperlink ref="D6" r:id="rId4"/>
+    <hyperlink ref="D5" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="800" verticalDpi="800" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="800" verticalDpi="800" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>